<commit_message>
Update Chrome Driver to 111
</commit_message>
<xml_diff>
--- a/2022_05.xlsx
+++ b/2022_05.xlsx
@@ -469,11 +469,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mon Jun 20 12:50:11 2022</t>
+          <t>Sat Mar 11 14:27:49 2023</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">

</xml_diff>